<commit_message>
chore: Add recursive call instead of listing all cellTypes
</commit_message>
<xml_diff>
--- a/dataframe-excel/src/test/resources/formula_cell.xlsx
+++ b/dataframe-excel/src/test/resources/formula_cell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\outros\kotlin\dataframe\dataframe-excel\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A18A239-E82C-4084-B918-E2D4868F5A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7D82E0-B951-4368-8BE7-A40075C572A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88D68A35-3722-406A-A299-4926B4CE1C69}"/>
   </bookViews>
@@ -41,13 +41,13 @@
     <t>Number</t>
   </si>
   <si>
-    <t>Greather than 5</t>
+    <t>Multiplied by 10</t>
   </si>
   <si>
-    <t>Divide by 5</t>
+    <t>Greater than 5</t>
   </si>
   <si>
-    <t>Multiplied by 10</t>
+    <t>Divided by 5</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,13 +412,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>